<commit_message>
[박청아] Add - [Item] 매대 SlotData 변경 시 Item View 처리, Item BP 생성, 테이블 값 적용
</commit_message>
<xml_diff>
--- a/Content/TableData/BasePath_BP_File.xlsx
+++ b/Content/TableData/BasePath_BP_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capark2690\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EF9B54-D988-49E3-9680-C73E43844EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CB5C6E-7B1E-4EE0-9F9F-F55AB2FD4390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="164">
   <si>
     <t>UI/Widget/InMarket</t>
   </si>
@@ -401,19 +401,129 @@
     <t>BP_SlotActor_4x4</t>
   </si>
   <si>
-    <t>BP_Item</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>BP_Rack_4x2_A</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BP_SnackA</t>
+  </si>
+  <si>
+    <t>BP_SnackB</t>
+  </si>
+  <si>
+    <t>BP_SnackC</t>
+  </si>
+  <si>
+    <t>BP_GoodsA</t>
+  </si>
+  <si>
+    <t>BP_GoodsB</t>
+  </si>
+  <si>
+    <t>BP_GoodsC</t>
+  </si>
+  <si>
+    <t>BP_GoodsD</t>
+  </si>
+  <si>
+    <t>BP_GoodsE</t>
+  </si>
+  <si>
+    <t>BP_GoodsF</t>
+  </si>
+  <si>
+    <t>BP_GoodsG</t>
+  </si>
+  <si>
+    <t>BP_GoodsH</t>
+  </si>
+  <si>
+    <t>BP_GoodsI</t>
+  </si>
+  <si>
+    <t>BP_Apple</t>
+  </si>
+  <si>
+    <t>BP_Orange</t>
+  </si>
+  <si>
+    <t>BP_FruitA</t>
+  </si>
+  <si>
+    <t>BP_FruitB</t>
+  </si>
+  <si>
+    <t>BP_GreenOnion</t>
+  </si>
+  <si>
+    <t>BP_Fish</t>
+  </si>
+  <si>
+    <t>BP_FishA</t>
+  </si>
+  <si>
+    <t>BP_FishB</t>
+  </si>
+  <si>
+    <t>BP_FishC</t>
+  </si>
+  <si>
+    <t>BP_FishD</t>
+  </si>
+  <si>
+    <t>BP_Dumpling</t>
+  </si>
+  <si>
+    <t>BP_Hamburger</t>
+  </si>
+  <si>
+    <t>BP_IceCream</t>
+  </si>
+  <si>
+    <t>BP_JuiceA</t>
+  </si>
+  <si>
+    <t>BP_JuiceB</t>
+  </si>
+  <si>
+    <t>BP_JuiceC</t>
+  </si>
+  <si>
+    <t>BP_JuiceD</t>
+  </si>
+  <si>
+    <t>BP_JuiceE</t>
+  </si>
+  <si>
+    <t>BP_JuiceF</t>
+  </si>
+  <si>
+    <t>BP_MilkA</t>
+  </si>
+  <si>
+    <t>BP_MilkB</t>
+  </si>
+  <si>
+    <t>BP_MilkC</t>
+  </si>
+  <si>
+    <t>BP_MilkD</t>
+  </si>
+  <si>
+    <t>BP_MilkE</t>
+  </si>
+  <si>
+    <t>BP_MilkF</t>
+  </si>
+  <si>
+    <t>BP_MilkG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -438,6 +548,12 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1048,10 +1164,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C48"/>
+  <dimension ref="A1:C85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:XFD47"/>
+    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C86" sqref="C86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1421,7 +1537,7 @@
         <v>4001</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1580,13 +1696,420 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48">
-        <v>8001</v>
+        <v>8004</v>
       </c>
       <c r="B48">
         <v>8001</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>125</v>
+      <c r="C48" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>8005</v>
+      </c>
+      <c r="B49">
+        <v>8001</v>
+      </c>
+      <c r="C49" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>8006</v>
+      </c>
+      <c r="B50">
+        <v>8001</v>
+      </c>
+      <c r="C50" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>8007</v>
+      </c>
+      <c r="B51">
+        <v>8001</v>
+      </c>
+      <c r="C51" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>8008</v>
+      </c>
+      <c r="B52">
+        <v>8001</v>
+      </c>
+      <c r="C52" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>8009</v>
+      </c>
+      <c r="B53">
+        <v>8001</v>
+      </c>
+      <c r="C53" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>8010</v>
+      </c>
+      <c r="B54">
+        <v>8001</v>
+      </c>
+      <c r="C54" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>8011</v>
+      </c>
+      <c r="B55">
+        <v>8001</v>
+      </c>
+      <c r="C55" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>8012</v>
+      </c>
+      <c r="B56">
+        <v>8001</v>
+      </c>
+      <c r="C56" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>8013</v>
+      </c>
+      <c r="B57">
+        <v>8001</v>
+      </c>
+      <c r="C57" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>8014</v>
+      </c>
+      <c r="B58">
+        <v>8001</v>
+      </c>
+      <c r="C58" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>8015</v>
+      </c>
+      <c r="B59">
+        <v>8001</v>
+      </c>
+      <c r="C59" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>8016</v>
+      </c>
+      <c r="B60">
+        <v>8001</v>
+      </c>
+      <c r="C60" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>8017</v>
+      </c>
+      <c r="B61">
+        <v>8001</v>
+      </c>
+      <c r="C61" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>8018</v>
+      </c>
+      <c r="B62">
+        <v>8001</v>
+      </c>
+      <c r="C62" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>8019</v>
+      </c>
+      <c r="B63">
+        <v>8001</v>
+      </c>
+      <c r="C63" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>8020</v>
+      </c>
+      <c r="B64">
+        <v>8001</v>
+      </c>
+      <c r="C64" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>8021</v>
+      </c>
+      <c r="B65">
+        <v>8001</v>
+      </c>
+      <c r="C65" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>8022</v>
+      </c>
+      <c r="B66">
+        <v>8001</v>
+      </c>
+      <c r="C66" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>8023</v>
+      </c>
+      <c r="B67">
+        <v>8001</v>
+      </c>
+      <c r="C67" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>8024</v>
+      </c>
+      <c r="B68">
+        <v>8001</v>
+      </c>
+      <c r="C68" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>8025</v>
+      </c>
+      <c r="B69">
+        <v>8001</v>
+      </c>
+      <c r="C69" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>8026</v>
+      </c>
+      <c r="B70">
+        <v>8001</v>
+      </c>
+      <c r="C70" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>8027</v>
+      </c>
+      <c r="B71">
+        <v>8001</v>
+      </c>
+      <c r="C71" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>8028</v>
+      </c>
+      <c r="B72">
+        <v>8001</v>
+      </c>
+      <c r="C72" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>8029</v>
+      </c>
+      <c r="B73">
+        <v>8001</v>
+      </c>
+      <c r="C73" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>8030</v>
+      </c>
+      <c r="B74">
+        <v>8001</v>
+      </c>
+      <c r="C74" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>8031</v>
+      </c>
+      <c r="B75">
+        <v>8001</v>
+      </c>
+      <c r="C75" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>8032</v>
+      </c>
+      <c r="B76">
+        <v>8001</v>
+      </c>
+      <c r="C76" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>8033</v>
+      </c>
+      <c r="B77">
+        <v>8001</v>
+      </c>
+      <c r="C77" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>8034</v>
+      </c>
+      <c r="B78">
+        <v>8001</v>
+      </c>
+      <c r="C78" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>8035</v>
+      </c>
+      <c r="B79">
+        <v>8001</v>
+      </c>
+      <c r="C79" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>8036</v>
+      </c>
+      <c r="B80">
+        <v>8001</v>
+      </c>
+      <c r="C80" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>8037</v>
+      </c>
+      <c r="B81">
+        <v>8001</v>
+      </c>
+      <c r="C81" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>8038</v>
+      </c>
+      <c r="B82">
+        <v>8001</v>
+      </c>
+      <c r="C82" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>8039</v>
+      </c>
+      <c r="B83">
+        <v>8001</v>
+      </c>
+      <c r="C83" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>8040</v>
+      </c>
+      <c r="B84">
+        <v>8001</v>
+      </c>
+      <c r="C84" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>8041</v>
+      </c>
+      <c r="B85">
+        <v>8001</v>
+      </c>
+      <c r="C85" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
박청아 Add - [AI] Staff, Customer AI Character 추가 / Staff 스폰
</commit_message>
<xml_diff>
--- a/Content/TableData/BasePath_BP_File.xlsx
+++ b/Content/TableData/BasePath_BP_File.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\capark2690\ProjectMS\Content\TableData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59CB5C6E-7B1E-4EE0-9F9F-F55AB2FD4390}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793D6EAA-56E7-48F7-B738-43EBA08F7483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25830" yWindow="3165" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BasePath_Directory" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="166">
   <si>
     <t>UI/Widget/InMarket</t>
   </si>
@@ -517,13 +517,21 @@
   </si>
   <si>
     <t>BP_MilkG</t>
+  </si>
+  <si>
+    <t>BP_StaffAICharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BP_CustomerAICharacter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -548,12 +556,6 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="돋움"/>
-      <family val="3"/>
-      <charset val="129"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1164,10 +1166,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:C85"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C86" sqref="C86"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A88" sqref="A88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2110,6 +2112,28 @@
       </c>
       <c r="C85" t="s">
         <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>9001</v>
+      </c>
+      <c r="B86">
+        <v>9001</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>9002</v>
+      </c>
+      <c r="B87">
+        <v>9001</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>